<commit_message>
finished fieldnotes & refactored
</commit_message>
<xml_diff>
--- a/01_background/Intervention Tracker - Post Intervention ONLY.xlsx
+++ b/01_background/Intervention Tracker - Post Intervention ONLY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\data.ucdenver.pvt\dept\SOM\FM\FM\Data_Management_Team\norc\01_background\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{403870B0-5CA2-4F09-BFA3-A12D3E2154CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0E28CD-41D2-4892-B89D-1D5D9A811C64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1815,7 +1815,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>